<commit_message>
Fast LED performance measurements
</commit_message>
<xml_diff>
--- a/Documentation/Measurements.xlsx
+++ b/Documentation/Measurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignatev\Documents\Projects\Fork\ResearchProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259164F7-9E9D-429A-984A-64B2D455F1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478C53B0-C73A-4907-9C03-A51E36C24424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10755" yWindow="2535" windowWidth="23310" windowHeight="15345" tabRatio="514" xr2:uid="{07024F4D-E5C7-4B8A-AB6A-143DE046C366}"/>
+    <workbookView xWindow="13440" yWindow="930" windowWidth="23310" windowHeight="15345" tabRatio="514" activeTab="1" xr2:uid="{07024F4D-E5C7-4B8A-AB6A-143DE046C366}"/>
   </bookViews>
   <sheets>
     <sheet name="FPGA" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>LEDs</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>Expenses</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>dT</t>
+  </si>
+  <si>
+    <t>Comparison of MCU controllers performance at SCLK = 1 MHz</t>
+  </si>
+  <si>
+    <t>Comparison of MCU controllers performance at LEDs = 30</t>
   </si>
 </sst>
 </file>
@@ -2403,6 +2418,1039 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>GPIO</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>FPGA!$B$5:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MCU!$C$5:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1449.2753623188407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>833.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>440.52863436123346</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>303.03030303030306</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>230.94688221709006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>184.16206261510129</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>153.84615384615387</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6048-4D97-B4EB-D476E7F48790}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>SPI</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>FPGA!$B$5:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MCU!$D$5:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1470.5882352941176</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>851.78875638841566</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>434.78260869565224</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>295.85798816568047</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>224.71910112359549</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>180.83182640144665</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>151.28593040847198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6048-4D97-B4EB-D476E7F48790}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1391260000"/>
+        <c:axId val="1388076240"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1391260000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>LEDs axis</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.5059861703588332"/>
+              <c:y val="0.91364877409052792"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1388076240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1388076240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Controller's</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> f</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>ramerate, Hz</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1391260000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="0"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>GPIO</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>FPGA!$J$5:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MCU!$K$5:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>833</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>833</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0AA4-4334-BC55-B0A17A5C1CFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>SPI</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>FPGA!$J$5:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MCU!$L$5:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>852</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2083</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0AA4-4334-BC55-B0A17A5C1CFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1391260000"/>
+        <c:axId val="1388076240"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1391260000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>CLK axis, MHz</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.5059861703588332"/>
+              <c:y val="0.91364877409052792"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1388076240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1388076240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Controller's</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> f</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>ramerate, Hz</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1391260000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="0"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -2477,6 +3525,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2994,6 +4079,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3656,6 +5257,87 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF92557E-E9E3-48D5-8895-4DBD3A39C9EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2B0D97B-1D92-4EA8-AAB9-B31E9D2BBB69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3963,8 +5645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A9648D-BF06-4D48-9391-82B9A0717805}">
   <dimension ref="B2:L123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4324,12 +6006,295 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC4A024-CB98-4091-A228-30579E405E35}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:L123"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="8" width="11.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="5">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5">
+        <f>1/F5 * 1000</f>
+        <v>1449.2753623188407</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" ref="D5:D11" si="0">1/G5*1000</f>
+        <v>1470.5882352941176</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.68</v>
+      </c>
+      <c r="J5" s="5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5">
+        <v>833</v>
+      </c>
+      <c r="L5" s="5">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6" s="5">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5">
+        <f t="shared" ref="C6:C11" si="1">1/F6 * 1000</f>
+        <v>833.33333333333337</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>851.78875638841566</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1.1739999999999999</v>
+      </c>
+      <c r="J6" s="5">
+        <v>6</v>
+      </c>
+      <c r="K6" s="5">
+        <v>833</v>
+      </c>
+      <c r="L6" s="5">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="5">
+        <v>60</v>
+      </c>
+      <c r="C7" s="5">
+        <f t="shared" si="1"/>
+        <v>440.52863436123346</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>434.78260869565224</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2.27</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="5">
+        <v>90</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" si="1"/>
+        <v>303.03030303030306</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>295.85798816568047</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="G8" s="4">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="5">
+        <v>120</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" si="1"/>
+        <v>230.94688221709006</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>224.71910112359549</v>
+      </c>
+      <c r="F9" s="4">
+        <v>4.33</v>
+      </c>
+      <c r="G9" s="4">
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="5">
+        <v>150</v>
+      </c>
+      <c r="C10" s="5">
+        <f t="shared" si="1"/>
+        <v>184.16206261510129</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
+        <v>180.83182640144665</v>
+      </c>
+      <c r="F10" s="4">
+        <v>5.43</v>
+      </c>
+      <c r="G10" s="4">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="5">
+        <v>180</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="1"/>
+        <v>153.84615384615387</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>151.28593040847198</v>
+      </c>
+      <c r="F11" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="G11" s="4">
+        <v>6.61</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+    </row>
+    <row r="75" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B75" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B94" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B108" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B122" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B123" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>